<commit_message>
#31 Added InTableOptionDefinition. Added readContext methods in XlBeanReader.
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/reader/TestBook_option.xlsx
+++ b/src/test/resources/org/xlbean/reader/TestBook_option.xlsx
@@ -1,32 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC702ED0-EC72-45C9-8959-5D53D3467398}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743D1196-0FA4-4260-940E-9E732ED574F2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8243" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5808" yWindow="0" windowWidth="19200" windowHeight="8244" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="limit" sheetId="3" r:id="rId1"/>
     <sheet name="offset" sheetId="7" r:id="rId2"/>
+    <sheet name="inTableOptions" sheetId="8" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -48,6 +55,50 @@
   </si>
   <si>
     <t>optionsOffset#~</t>
+  </si>
+  <si>
+    <t>optionsInTable#field1</t>
+  </si>
+  <si>
+    <t>optionsInTable#field2</t>
+  </si>
+  <si>
+    <t>optionsInTable?customType</t>
+  </si>
+  <si>
+    <t>optionsInTable#~</t>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hoge</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>fuga</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>single</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>single?type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionsInTable?type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>single?custom</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>test value for custom option</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -71,12 +122,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,8 +156,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -417,13 +486,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="1.25" customWidth="1"/>
+    <col min="2" max="2" width="1.19921875" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -431,7 +500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -439,82 +508,82 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C12">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C13">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C14">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C15">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C16">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.7">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C17">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.7">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C18">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.7">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C19">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.7">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C20">
         <v>17</v>
       </c>
@@ -530,18 +599,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDDA968-1B28-4738-AFD0-E2D80CC6A6CD}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.9375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.25" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.19921875" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -557,82 +626,82 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C12">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C13">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C14">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C15">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C16">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.7">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C17">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.7">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C18">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.7">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C19">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.7">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C20">
         <v>17</v>
       </c>
@@ -642,4 +711,194 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D9689B-68B4-4F4B-A7B6-7E6CA45994A3}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="25.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="C2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="C5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <f>E11+100</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" ref="F12:F18" si="0">E12+100</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E14" s="2">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E16" s="2">
+        <v>6</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="E17" s="2">
+        <v>7</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="E18" s="2">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#33 Fixed NPE in BeanConverterImpl
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/reader/TestBook_option.xlsx
+++ b/src/test/resources/org/xlbean/reader/TestBook_option.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743D1196-0FA4-4260-940E-9E732ED574F2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFF7EFD-F952-422C-8EB1-6CE7779FC212}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5808" yWindow="0" windowWidth="19200" windowHeight="8244" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7260" yWindow="0" windowWidth="19200" windowHeight="8244" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="limit" sheetId="3" r:id="rId1"/>
     <sheet name="offset" sheetId="7" r:id="rId2"/>
     <sheet name="inTableOptions" sheetId="8" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -98,6 +98,22 @@
   </si>
   <si>
     <t>test value for custom option</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionToOtherDirection</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionToOtherDirection?testOption</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>value for option</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -122,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +157,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -156,7 +178,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -164,6 +186,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -715,10 +740,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D9689B-68B4-4F4B-A7B6-7E6CA45994A3}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -727,7 +752,7 @@
     <col min="5" max="6" width="21.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -740,13 +765,21 @@
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -756,8 +789,10 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -767,13 +802,17 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C5" s="1"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -783,12 +822,16 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -799,8 +842,10 @@
         <v>10</v>
       </c>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -813,12 +858,16 @@
       <c r="F9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -832,8 +881,10 @@
         <f>E11+100</f>
         <v>101</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E12" s="2">
         <v>2</v>
       </c>
@@ -841,8 +892,10 @@
         <f t="shared" ref="F12:F18" si="0">E12+100</f>
         <v>102</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E13" s="2">
         <v>3</v>
       </c>
@@ -850,8 +903,10 @@
         <f t="shared" si="0"/>
         <v>103</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E14" s="2">
         <v>4</v>
       </c>
@@ -859,8 +914,10 @@
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E15" s="2">
         <v>5</v>
       </c>
@@ -868,8 +925,10 @@
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E16" s="2">
         <v>6</v>
       </c>
@@ -877,8 +936,10 @@
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E17" s="2">
         <v>7</v>
       </c>
@@ -886,14 +947,40 @@
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E18" s="2">
         <v>8</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="0"/>
         <v>108</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#40 Fixed SingleDefinition#merge bug
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/reader/TestBook_option.xlsx
+++ b/src/test/resources/org/xlbean/reader/TestBook_option.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFF7EFD-F952-422C-8EB1-6CE7779FC212}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E53299A-8132-41B0-8FFF-2BE2CF14B960}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="0" windowWidth="19200" windowHeight="8244" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10164" yWindow="0" windowWidth="19200" windowHeight="8244" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="limit" sheetId="3" r:id="rId1"/>
     <sheet name="offset" sheetId="7" r:id="rId2"/>
     <sheet name="inTableOptions" sheetId="8" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -114,6 +115,46 @@
   </si>
   <si>
     <t>value for option</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionOnColumn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionOnColumn?testOption=testValue</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionOnColumnTable#test2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionOnColumnTable#test1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bbb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ccc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ddd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>eee</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionOnColumnTable?anotherOption=anotherValue&amp;oneMoreOption=someValue#~</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -742,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D9689B-68B4-4F4B-A7B6-7E6CA45994A3}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -988,4 +1029,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E0622A-FB0E-4C51-84B9-FC88D3CF6178}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="76.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="26.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed TableDefinitionBuilder not to add column options to table
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/reader/TestBook_option.xlsx
+++ b/src/test/resources/org/xlbean/reader/TestBook_option.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E53299A-8132-41B0-8FFF-2BE2CF14B960}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BFA05F-AC53-481B-AE5C-732BA3DE5DA7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10164" yWindow="0" windowWidth="19200" windowHeight="8244" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13068" yWindow="0" windowWidth="19200" windowHeight="8244" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="limit" sheetId="3" r:id="rId1"/>
     <sheet name="offset" sheetId="7" r:id="rId2"/>
     <sheet name="inTableOptions" sheetId="8" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId4"/>
+    <sheet name="optionOnColumn" sheetId="9" r:id="rId4"/>
+    <sheet name="optionForTableAndColumn" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -155,6 +156,34 @@
   </si>
   <si>
     <t>optionOnColumnTable?anotherOption=anotherValue&amp;oneMoreOption=someValue#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionForTableAndColumn001?opt1=val1#col1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionForTableAndColumn001#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionForTableAndColumn002#col1?opt1=val1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionForTableAndColumn002#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionForTableAndColumn002#col2?opt2=val2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionForTableAndColumn003#col1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optionForTableAndColumn003?opt3=val3#~</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1035,7 +1064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E0622A-FB0E-4C51-84B9-FC88D3CF6178}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1092,4 +1121,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B6981D-F643-4E7E-ACE2-05DF4AE4312B}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="40.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.8984375" customWidth="1"/>
+    <col min="3" max="3" width="39.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.8984375" customWidth="1"/>
+    <col min="5" max="6" width="42.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.8984375" customWidth="1"/>
+    <col min="8" max="8" width="32.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#65 Updated Options structure to be able to have globalOptions
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/reader/TestBook_option.xlsx
+++ b/src/test/resources/org/xlbean/reader/TestBook_option.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA34104E-0445-4530-9D81-1CA18B82E544}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D025CDF0-C458-471E-9344-13B6AD7983DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="-108" windowWidth="29448" windowHeight="17496" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="-108" windowWidth="29448" windowHeight="17496" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="limit" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="inTableOptions" sheetId="8" r:id="rId3"/>
     <sheet name="optionOnColumn" sheetId="9" r:id="rId4"/>
     <sheet name="optionForTableAndColumn" sheetId="10" r:id="rId5"/>
+    <sheet name="layeredOption" sheetId="11" r:id="rId6"/>
+    <sheet name="layeredOptionActual" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -183,6 +185,82 @@
   </si>
   <si>
     <t>optionsInTable?readAs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>####?global=val1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dddd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredaaa?single=val2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredtable#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredtable2#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredbbb?global=val9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredaaa, layeredbbb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>eeee</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredtable2?global=val99#col</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredtable2#col?global=val999</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredtable?table=val3#column1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredtable#column3?table=val9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredtable#column2?column=val4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>####?readAs=text</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredAct</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;- this to be "1" and not "1.0"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredActTable#col1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredActTable?fieldType=int#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>layeredActTable#col2?fieldType=boolean</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -811,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D9689B-68B4-4F4B-A7B6-7E6CA45994A3}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1190,4 +1268,187 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FD701C-CE08-44CE-A461-B0F060215108}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="0.796875" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.69921875" customWidth="1"/>
+    <col min="6" max="6" width="29.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.8984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0.796875" customWidth="1"/>
+    <col min="10" max="10" width="29.09765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>111</v>
+      </c>
+      <c r="G5">
+        <v>222</v>
+      </c>
+      <c r="H5">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F6">
+        <v>444</v>
+      </c>
+      <c r="G6">
+        <v>555</v>
+      </c>
+      <c r="H6">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C27FB74-DAA5-43C1-BF71-EBF44478A199}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>